<commit_message>
Check to fix null / empty string
</commit_message>
<xml_diff>
--- a/Company1.xlsx
+++ b/Company1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="224">
   <si>
     <t>addresslines</t>
   </si>
@@ -61,11 +61,6 @@
   </si>
   <si>
     <t>S9 2DD</t>
-  </si>
-  <si>
-    <t>Rotherham Area Business Centre
-PO Box 36
-High Street</t>
   </si>
   <si>
     <t>Rotherham</t>
@@ -1559,7 +1554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1574,10 +1569,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" t="s">
         <v>223</v>
-      </c>
-      <c r="B1" t="s">
-        <v>224</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1589,21 +1584,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1614,13 +1604,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1631,13 +1621,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1648,13 +1638,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
         <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1665,13 +1655,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
         <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1682,13 +1672,13 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1699,13 +1689,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
         <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1716,7 +1706,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -1733,13 +1723,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1750,13 +1740,13 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1767,13 +1757,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1784,13 +1774,13 @@
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1801,13 +1791,13 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
         <v>38</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>39</v>
-      </c>
-      <c r="E14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1818,13 +1808,13 @@
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
         <v>41</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>42</v>
-      </c>
-      <c r="E15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -1835,13 +1825,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
         <v>44</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>45</v>
-      </c>
-      <c r="E16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1852,13 +1842,13 @@
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
         <v>47</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>48</v>
-      </c>
-      <c r="E17" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1869,13 +1859,13 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -1886,13 +1876,13 @@
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
         <v>52</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>53</v>
-      </c>
-      <c r="E19" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1903,13 +1893,13 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
         <v>55</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>56</v>
-      </c>
-      <c r="E20" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1920,7 +1910,7 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
         <v>3</v>
@@ -1937,13 +1927,13 @@
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" t="s">
         <v>48</v>
-      </c>
-      <c r="E22" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1954,13 +1944,13 @@
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
         <v>60</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>61</v>
-      </c>
-      <c r="E23" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1971,41 +1961,41 @@
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
         <v>63</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>64</v>
-      </c>
-      <c r="C25" t="s">
-        <v>65</v>
       </c>
       <c r="D25" t="s">
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
         <v>63</v>
       </c>
-      <c r="B26" t="s">
-        <v>64</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" t="s">
         <v>3</v>
@@ -2013,781 +2003,781 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
         <v>68</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>69</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>70</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>71</v>
-      </c>
-      <c r="E27" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
         <v>73</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
         <v>77</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" t="s">
         <v>81</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" t="s">
         <v>83</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>84</v>
-      </c>
-      <c r="E30" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s">
         <v>86</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
       </c>
       <c r="E31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" t="s">
         <v>90</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" t="s">
         <v>92</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>93</v>
-      </c>
-      <c r="E32" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
         <v>95</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="D33" t="s">
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" t="s">
         <v>95</v>
       </c>
-      <c r="B34" t="s">
-        <v>96</v>
-      </c>
       <c r="C34" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" t="s">
         <v>99</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>100</v>
-      </c>
-      <c r="E34" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" t="s">
         <v>95</v>
       </c>
-      <c r="B35" t="s">
-        <v>96</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" t="s">
         <v>95</v>
       </c>
-      <c r="B36" t="s">
-        <v>96</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D36" t="s">
         <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" t="s">
         <v>106</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" t="s">
         <v>108</v>
-      </c>
-      <c r="D37" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" t="s">
         <v>110</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>111</v>
-      </c>
-      <c r="C38" t="s">
-        <v>112</v>
       </c>
       <c r="D38" t="s">
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" t="s">
         <v>114</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" t="s">
         <v>116</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>117</v>
-      </c>
-      <c r="E39" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" t="s">
         <v>119</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" t="s">
         <v>121</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>122</v>
-      </c>
-      <c r="E40" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" t="s">
         <v>124</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>125</v>
-      </c>
-      <c r="C41" t="s">
-        <v>126</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>127</v>
+      </c>
+      <c r="B42" t="s">
         <v>128</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" t="s">
         <v>130</v>
-      </c>
-      <c r="D42" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" t="s">
         <v>132</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>133</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>134</v>
-      </c>
-      <c r="D43" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>131</v>
+      </c>
+      <c r="B44" t="s">
         <v>132</v>
       </c>
-      <c r="B44" t="s">
-        <v>133</v>
-      </c>
       <c r="C44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D44" t="s">
         <v>136</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>137</v>
-      </c>
-      <c r="E44" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" t="s">
         <v>139</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>140</v>
-      </c>
-      <c r="C45" t="s">
-        <v>141</v>
       </c>
       <c r="D45" t="s">
         <v>8</v>
       </c>
       <c r="E45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46" t="s">
         <v>139</v>
       </c>
-      <c r="B46" t="s">
-        <v>140</v>
-      </c>
       <c r="C46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D46" t="s">
         <v>4</v>
       </c>
       <c r="E46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>138</v>
+      </c>
+      <c r="B47" t="s">
         <v>139</v>
       </c>
-      <c r="B47" t="s">
-        <v>140</v>
-      </c>
       <c r="C47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D47" t="s">
         <v>4</v>
       </c>
       <c r="E47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" t="s">
         <v>139</v>
       </c>
-      <c r="B48" t="s">
-        <v>140</v>
-      </c>
       <c r="C48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D48" t="s">
         <v>4</v>
       </c>
       <c r="E48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>138</v>
+      </c>
+      <c r="B49" t="s">
         <v>139</v>
       </c>
-      <c r="B49" t="s">
-        <v>140</v>
-      </c>
       <c r="C49" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>138</v>
+      </c>
+      <c r="B50" t="s">
         <v>139</v>
       </c>
-      <c r="B50" t="s">
-        <v>140</v>
-      </c>
       <c r="C50" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D50" t="s">
         <v>3</v>
       </c>
       <c r="E50" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" t="s">
         <v>139</v>
       </c>
-      <c r="B51" t="s">
-        <v>140</v>
-      </c>
       <c r="C51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
       </c>
       <c r="E51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>138</v>
+      </c>
+      <c r="B52" t="s">
         <v>139</v>
       </c>
-      <c r="B52" t="s">
-        <v>140</v>
-      </c>
       <c r="C52" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D52" t="s">
         <v>3</v>
       </c>
       <c r="E52" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>138</v>
+      </c>
+      <c r="B53" t="s">
         <v>139</v>
       </c>
-      <c r="B53" t="s">
-        <v>140</v>
-      </c>
       <c r="C53" t="s">
+        <v>156</v>
+      </c>
+      <c r="D53" t="s">
         <v>157</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>158</v>
-      </c>
-      <c r="E53" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>138</v>
+      </c>
+      <c r="B54" t="s">
         <v>139</v>
       </c>
-      <c r="B54" t="s">
-        <v>140</v>
-      </c>
       <c r="C54" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" t="s">
+        <v>52</v>
+      </c>
+      <c r="E54" t="s">
         <v>160</v>
-      </c>
-      <c r="D54" t="s">
-        <v>53</v>
-      </c>
-      <c r="E54" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" t="s">
         <v>162</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>163</v>
-      </c>
-      <c r="C55" t="s">
-        <v>164</v>
       </c>
       <c r="D55" t="s">
         <v>8</v>
       </c>
       <c r="E55" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>161</v>
+      </c>
+      <c r="B56" t="s">
         <v>162</v>
       </c>
-      <c r="B56" t="s">
-        <v>163</v>
-      </c>
       <c r="C56" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D56" t="s">
         <v>4</v>
       </c>
       <c r="E56" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>161</v>
+      </c>
+      <c r="B57" t="s">
         <v>162</v>
       </c>
-      <c r="B57" t="s">
-        <v>163</v>
-      </c>
       <c r="C57" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D57" t="s">
         <v>8</v>
       </c>
       <c r="E57" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>161</v>
+      </c>
+      <c r="B58" t="s">
         <v>162</v>
       </c>
-      <c r="B58" t="s">
-        <v>163</v>
-      </c>
       <c r="C58" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>161</v>
+      </c>
+      <c r="B59" t="s">
         <v>162</v>
       </c>
-      <c r="B59" t="s">
-        <v>163</v>
-      </c>
       <c r="C59" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D59" t="s">
         <v>3</v>
       </c>
       <c r="E59" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>173</v>
+      </c>
+      <c r="B60" t="s">
         <v>174</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>175</v>
-      </c>
-      <c r="C60" t="s">
-        <v>176</v>
       </c>
       <c r="D60" t="s">
         <v>4</v>
       </c>
       <c r="E60" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>177</v>
+      </c>
+      <c r="B61" t="s">
         <v>178</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="D61" t="s">
         <v>180</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>181</v>
-      </c>
-      <c r="E61" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>182</v>
+      </c>
+      <c r="B62" t="s">
         <v>183</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="D62" t="s">
         <v>185</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>186</v>
-      </c>
-      <c r="E62" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>182</v>
+      </c>
+      <c r="B63" t="s">
         <v>183</v>
       </c>
-      <c r="B63" t="s">
-        <v>184</v>
-      </c>
       <c r="C63" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D63" t="s">
         <v>188</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>189</v>
-      </c>
-      <c r="E63" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>182</v>
+      </c>
+      <c r="B64" t="s">
         <v>183</v>
       </c>
-      <c r="B64" t="s">
-        <v>184</v>
-      </c>
       <c r="C64" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D64" t="s">
         <v>191</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>192</v>
-      </c>
-      <c r="E64" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>193</v>
+      </c>
+      <c r="B65" t="s">
         <v>194</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>195</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>196</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>197</v>
-      </c>
-      <c r="E65" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>198</v>
+      </c>
+      <c r="B66" t="s">
         <v>199</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>200</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>201</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>202</v>
-      </c>
-      <c r="E66" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>198</v>
+      </c>
+      <c r="B67" t="s">
         <v>199</v>
       </c>
-      <c r="B67" t="s">
-        <v>200</v>
-      </c>
       <c r="C67" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D67" t="s">
+        <v>201</v>
+      </c>
+      <c r="E67" t="s">
         <v>204</v>
-      </c>
-      <c r="D67" t="s">
-        <v>202</v>
-      </c>
-      <c r="E67" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>198</v>
+      </c>
+      <c r="B68" t="s">
         <v>199</v>
       </c>
-      <c r="B68" t="s">
-        <v>200</v>
-      </c>
       <c r="C68" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
       </c>
       <c r="E68" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>207</v>
+      </c>
+      <c r="B69" t="s">
         <v>208</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>209</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>210</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>211</v>
-      </c>
-      <c r="E69" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>207</v>
+      </c>
+      <c r="B70" t="s">
         <v>208</v>
       </c>
-      <c r="B70" t="s">
-        <v>209</v>
-      </c>
       <c r="C70" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D70" t="s">
+        <v>210</v>
+      </c>
+      <c r="E70" t="s">
         <v>213</v>
-      </c>
-      <c r="D70" t="s">
-        <v>211</v>
-      </c>
-      <c r="E70" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>207</v>
+      </c>
+      <c r="B71" t="s">
         <v>208</v>
       </c>
-      <c r="B71" t="s">
-        <v>209</v>
-      </c>
       <c r="C71" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D71" t="s">
         <v>215</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>216</v>
-      </c>
-      <c r="E71" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>217</v>
+      </c>
+      <c r="B72" t="s">
         <v>218</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="D72" t="s">
         <v>220</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>221</v>
-      </c>
-      <c r="E72" t="s">
-        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>